<commit_message>
unit tests not passing
</commit_message>
<xml_diff>
--- a/tests/test_paklijsten/paklijst1.xlsx
+++ b/tests/test_paklijsten/paklijst1.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\HDS\2d_rectangle_packing\tests\test_paklijsten\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102D4F86-1190-415A-B637-5022D33D44D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="paklijst_zonder_opmaak" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Paklijst" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="paklijst_zonder_opmaak" sheetId="1" r:id="rId1"/>
+    <sheet name="Paklijst" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,64 +26,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="110">
-  <si>
-    <t xml:space="preserve">Aantal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omschrijving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breedte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lengte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orderdatum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coupage/Batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ordernummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Klantnaam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rolbreedte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kleur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kokos</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="111">
+  <si>
+    <t>Aantal</t>
+  </si>
+  <si>
+    <t>Merk</t>
+  </si>
+  <si>
+    <t>Omschrijving</t>
+  </si>
+  <si>
+    <t>Breedte</t>
+  </si>
+  <si>
+    <t>Lengte</t>
+  </si>
+  <si>
+    <t>Orderdatum</t>
+  </si>
+  <si>
+    <t>Coupage/Batch</t>
+  </si>
+  <si>
+    <t>Ordernummer</t>
+  </si>
+  <si>
+    <t>Klantnaam</t>
+  </si>
+  <si>
+    <t>Rolbreedte</t>
+  </si>
+  <si>
+    <t>Kleur</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Kokos</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet 50 x 80 cm_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Dings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">antraciet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. van de Venn</t>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>Mevr. Dings</t>
+  </si>
+  <si>
+    <t>antraciet</t>
+  </si>
+  <si>
+    <t>Dhr. van de Venn</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -89,10 +94,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. Siebers</t>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Dhr. Siebers</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -101,10 +106,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tandartsenpraktijk Jansen</t>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Tandartsenpraktijk Jansen</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -115,10 +120,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. van Hees</t>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Mevr. van Hees</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -129,7 +134,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">85</t>
+    <t>85</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -138,13 +143,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">98,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. Edens</t>
+    <t>98,5</t>
+  </si>
+  <si>
+    <t>81,5</t>
+  </si>
+  <si>
+    <t>Dhr. Edens</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -153,39 +158,39 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lash &amp; Brow Bar</t>
+    <t>197</t>
+  </si>
+  <si>
+    <t>Lash &amp; Brow Bar</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Grijs 60 x 80 cm_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Boers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grijs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. De Groot</t>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Mevr. Boers</t>
+  </si>
+  <si>
+    <t>grijs</t>
+  </si>
+  <si>
+    <t>Mevr. De Groot</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel 60 x 80 cm_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Beugels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">naturel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
+    <t>Mevr. Beugels</t>
+  </si>
+  <si>
+    <t>naturel</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel 60 x 80 cm_x000D_
@@ -193,7 +198,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Dhr. Venhorst</t>
+    <t>Dhr. Venhorst</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -202,10 +207,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. Van der Zwaag</t>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Dhr. Van der Zwaag</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -214,13 +219,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. de Ruijter</t>
+    <t>101</t>
+  </si>
+  <si>
+    <t>93,5</t>
+  </si>
+  <si>
+    <t>Mevr. de Ruijter</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -229,10 +234,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Valk</t>
+    <t>103</t>
+  </si>
+  <si>
+    <t>Mevr. Valk</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -241,10 +246,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Veltman</t>
+    <t>160</t>
+  </si>
+  <si>
+    <t>Mevr. Veltman</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -255,7 +260,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Groen</t>
+    <t>Mevr. Groen</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -264,13 +269,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">91,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. De vuyst</t>
+    <t>91,2</t>
+  </si>
+  <si>
+    <t>92,3</t>
+  </si>
+  <si>
+    <t>Dhr. De vuyst</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -279,10 +284,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Bongertman</t>
+    <t>127</t>
+  </si>
+  <si>
+    <t>Mevr. Bongertman</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -291,13 +296,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">141,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. de Bruin</t>
+    <t>141,3</t>
+  </si>
+  <si>
+    <t>60,3</t>
+  </si>
+  <si>
+    <t>Mevr. de Bruin</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -306,10 +311,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Zeevat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zwart</t>
+    <t>Mevr. Zeevat</t>
+  </si>
+  <si>
+    <t>zwart</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -318,7 +323,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Michelle’s schoonmaakbedrijf</t>
+    <t>Michelle’s schoonmaakbedrijf</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -327,7 +332,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Cortlever</t>
+    <t>Mevr. Cortlever</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -336,10 +341,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">72,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. wiebenga</t>
+    <t>72,5</t>
+  </si>
+  <si>
+    <t>Mevr. wiebenga</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -350,10 +355,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Dubois</t>
+    <t>113</t>
+  </si>
+  <si>
+    <t>Mevr. Dubois</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -362,10 +367,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">38,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Thys</t>
+    <t>38,3</t>
+  </si>
+  <si>
+    <t>Mevr. Thys</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -376,13 +381,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. Rops</t>
+    <t>68</t>
+  </si>
+  <si>
+    <t>104,5</t>
+  </si>
+  <si>
+    <t>Dhr. Rops</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -393,13 +398,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Haan</t>
+    <t>78</t>
+  </si>
+  <si>
+    <t>48,5</t>
+  </si>
+  <si>
+    <t>Mevr. Haan</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -408,7 +413,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Huisman</t>
+    <t>Mevr. Huisman</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -417,13 +422,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">86,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Pijnenburg</t>
+    <t>86,5</t>
+  </si>
+  <si>
+    <t>48,3</t>
+  </si>
+  <si>
+    <t>Mevr. Pijnenburg</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -432,7 +437,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">87</t>
+    <t>87</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -443,25 +448,26 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Harsch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Batch/Coupage</t>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Mevr. Harsch</t>
+  </si>
+  <si>
+    <t>Batch/Coupage</t>
+  </si>
+  <si>
+    <t>Materiaal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -471,28 +477,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -509,1396 +500,1730 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:K33" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabel1" displayName="Tabel1" ref="A1:K33" totalsRowShown="0">
+  <autoFilter ref="A1:K33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Aantal"/>
-    <tableColumn id="2" name="Merk"/>
-    <tableColumn id="3" name="Omschrijving"/>
-    <tableColumn id="4" name="Breedte"/>
-    <tableColumn id="5" name="Lengte"/>
-    <tableColumn id="6" name="Orderdatum"/>
-    <tableColumn id="7" name="Batch/Coupage"/>
-    <tableColumn id="8" name="Ordernummer"/>
-    <tableColumn id="9" name="Klantnaam"/>
-    <tableColumn id="10" name="Rolbreedte"/>
-    <tableColumn id="11" name="Kleur"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aantal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Merk"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Omschrijving"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Breedte"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Lengte"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Orderdatum"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Batch/Coupage"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ordernummer"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Klantnaam"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Rolbreedte"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Kleur"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
+    <col min="1" max="1" width="6.5546875"/>
+    <col min="2" max="2" width="6.21875"/>
+    <col min="3" max="3" width="53.88671875"/>
+    <col min="4" max="4" width="8"/>
+    <col min="5" max="5" width="6.88671875"/>
+    <col min="6" max="6" width="11.5546875"/>
+    <col min="7" max="7" width="14.33203125"/>
+    <col min="8" max="8" width="13.6640625"/>
+    <col min="9" max="9" width="27.77734375"/>
+    <col min="10" max="10" width="10.77734375"/>
+    <col min="11" max="11" width="8.6640625"/>
+    <col min="12" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="L1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>80</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="0" t="n">
+      <c r="F2">
+        <v>44176</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
         <v>120344307</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K2" s="0" t="s">
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>80</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="F3">
+        <v>44176</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
         <v>120344364</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K3" s="0" t="s">
+      <c r="J3">
+        <v>100</v>
+      </c>
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>74</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>44146</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
         <v>120344112</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K4" s="0" t="s">
+      <c r="J4">
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="0" t="n">
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>44176</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
         <v>120344352</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K5" s="0" t="s">
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="K5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>60</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="0" t="n">
+      <c r="F6">
+        <v>44176</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
         <v>120344308</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K6" s="0" t="s">
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="K6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="L6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>90</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="F7">
+        <v>44176</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
         <v>120344352</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K7" s="0" t="s">
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="0" t="s">
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8">
         <v>44146</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
         <v>120344094</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K8" s="0" t="s">
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9">
         <v>105</v>
       </c>
-      <c r="F9" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="0" t="n">
+      <c r="F9">
+        <v>44176</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
         <v>120344255</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9">
         <v>200</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="L9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10">
         <v>80</v>
       </c>
-      <c r="F10" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="0" t="n">
+      <c r="F10">
+        <v>44176</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10">
         <v>120344196</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K10" s="0" t="s">
+      <c r="J10">
+        <v>100</v>
+      </c>
+      <c r="K10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="L10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11">
         <v>80</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="0" t="n">
+      <c r="F11">
+        <v>44176</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
         <v>120344195</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K11" s="0" t="s">
+      <c r="J11">
+        <v>100</v>
+      </c>
+      <c r="K11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="L11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12">
         <v>80</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="0" t="n">
+      <c r="F12">
+        <v>44176</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12">
         <v>120344184</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K12" s="0" t="s">
+      <c r="J12">
+        <v>100</v>
+      </c>
+      <c r="K12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="L12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13">
         <v>80</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="0" t="n">
+      <c r="F13">
+        <v>44176</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13">
         <v>120344135</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K13" s="0" t="s">
+      <c r="J13">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="L13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14">
         <v>75</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="0" t="n">
+      <c r="F14">
+        <v>44176</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14">
         <v>120344129</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K14" s="0" t="s">
+      <c r="J14">
+        <v>100</v>
+      </c>
+      <c r="K14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="L14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="0" t="n">
+      <c r="F15">
+        <v>44176</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15">
         <v>120344369</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K15" s="0" t="s">
+      <c r="J15">
+        <v>100</v>
+      </c>
+      <c r="K15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="L15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16">
         <v>85</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="0" t="n">
+      <c r="F16">
+        <v>44176</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16">
         <v>120344330</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K16" s="0" t="s">
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="L16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17">
         <v>95</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17">
         <v>44146</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="0" t="n">
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17">
         <v>120344100</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K17" s="0" t="s">
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="L17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18">
         <v>120</v>
       </c>
-      <c r="F18" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="0" t="n">
+      <c r="F18">
+        <v>44176</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18">
         <v>120344340</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K18" s="0" t="s">
+      <c r="J18">
+        <v>100</v>
+      </c>
+      <c r="K18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="L18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="0" t="n">
+      <c r="F19">
+        <v>44176</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
         <v>120344295</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K19" s="0" t="s">
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="0" t="s">
+      <c r="L19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20">
         <v>173</v>
       </c>
-      <c r="F20" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="0" t="n">
+      <c r="F20">
+        <v>44176</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20">
         <v>120344266</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" t="s">
         <v>69</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20">
         <v>200</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="K20" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="L20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="0" t="n">
+      <c r="F21">
+        <v>44176</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21">
         <v>120344324</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" t="s">
         <v>73</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21">
         <v>200</v>
       </c>
-      <c r="K21" s="0" t="s">
+      <c r="K21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="0" t="s">
+      <c r="L21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="0" t="n">
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>44176</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22">
         <v>120344293</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="I22" t="s">
         <v>75</v>
       </c>
-      <c r="J22" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K22" s="0" t="s">
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="K22" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="0" t="s">
+      <c r="L22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23">
         <v>120</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="0" t="n">
+      <c r="F23">
+        <v>44176</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23">
         <v>120344333</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="I23" t="s">
         <v>78</v>
       </c>
-      <c r="J23" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K23" s="0" t="s">
+      <c r="J23">
+        <v>100</v>
+      </c>
+      <c r="K23" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="0" t="s">
+      <c r="L23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24">
         <v>60</v>
       </c>
-      <c r="F24" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="0" t="n">
+      <c r="F24">
+        <v>44176</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24">
         <v>120344254</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" t="s">
         <v>80</v>
       </c>
-      <c r="J24" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K24" s="0" t="s">
+      <c r="J24">
+        <v>100</v>
+      </c>
+      <c r="K24" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="0" t="s">
+      <c r="L24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" t="s">
         <v>82</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25">
         <v>44146</v>
       </c>
-      <c r="G25" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="0" t="n">
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25">
         <v>120343858</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="I25" t="s">
         <v>83</v>
       </c>
-      <c r="J25" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K25" s="0" t="s">
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="0" t="s">
+      <c r="L25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26">
         <v>73</v>
       </c>
-      <c r="F26" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="0" t="n">
+      <c r="F26">
+        <v>44176</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26">
         <v>120344345</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I26" t="s">
         <v>86</v>
       </c>
-      <c r="J26" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K26" s="0" t="s">
+      <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="0" t="s">
+      <c r="L26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27">
         <v>58</v>
       </c>
-      <c r="F27" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="0" t="n">
+      <c r="F27">
+        <v>44176</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27">
         <v>120344250</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I27" t="s">
         <v>89</v>
       </c>
-      <c r="J27" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K27" s="0" t="s">
+      <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="K27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="0" t="s">
+      <c r="L27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="0" t="n">
+      <c r="F28">
+        <v>44176</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28">
         <v>120344320</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="I28" t="s">
         <v>93</v>
       </c>
-      <c r="J28" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K28" s="0" t="s">
+      <c r="J28">
+        <v>100</v>
+      </c>
+      <c r="K28" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="L28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29">
         <v>44146</v>
       </c>
-      <c r="G29" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="0" t="n">
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29">
         <v>120343945</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="I29" t="s">
         <v>97</v>
       </c>
-      <c r="J29" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K29" s="0" t="s">
+      <c r="J29">
+        <v>100</v>
+      </c>
+      <c r="K29" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="0" t="s">
+      <c r="L29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30">
         <v>60</v>
       </c>
-      <c r="F30" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="0" t="n">
+      <c r="F30">
+        <v>44176</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30">
         <v>120344313</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="I30" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K30" s="0" t="s">
+      <c r="J30">
+        <v>100</v>
+      </c>
+      <c r="K30" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="0" t="s">
+      <c r="L30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" t="s">
         <v>102</v>
       </c>
-      <c r="F31" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="0" t="n">
+      <c r="F31">
+        <v>44176</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31">
         <v>120344186</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="I31" t="s">
         <v>103</v>
       </c>
-      <c r="J31" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K31" s="0" t="s">
+      <c r="J31">
+        <v>100</v>
+      </c>
+      <c r="K31" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="0" t="s">
+      <c r="L31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32">
         <v>73</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="0" t="n">
+      <c r="F32">
+        <v>44176</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32">
         <v>120344345</v>
       </c>
-      <c r="I32" s="0" t="s">
+      <c r="I32" t="s">
         <v>86</v>
       </c>
-      <c r="J32" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K32" s="0" t="s">
+      <c r="J32">
+        <v>100</v>
+      </c>
+      <c r="K32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="0" t="s">
+      <c r="L32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33">
         <v>170</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33">
         <v>44146</v>
       </c>
-      <c r="G33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="0" t="n">
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33">
         <v>120343922</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="I33" t="s">
         <v>108</v>
       </c>
-      <c r="J33" s="0" t="n">
+      <c r="J33">
         <v>200</v>
       </c>
-      <c r="K33" s="0" t="s">
+      <c r="K33" t="s">
         <v>76</v>
       </c>
+      <c r="L33" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="3" width="9.04591836734694"/>
+    <col min="1" max="1" width="8" style="2"/>
+    <col min="2" max="2" width="15.6640625" style="3"/>
+    <col min="3" max="3" width="42.5546875" style="3"/>
+    <col min="4" max="4" width="9.44140625" style="4"/>
+    <col min="5" max="5" width="8.33203125" style="3"/>
+    <col min="6" max="6" width="12.77734375" style="3"/>
+    <col min="7" max="7" width="14.6640625" style="5"/>
+    <col min="8" max="8" width="14.44140625" style="5"/>
+    <col min="9" max="9" width="27.109375" style="3"/>
+    <col min="10" max="1025" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1933,7 +2258,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -1946,29 +2271,29 @@
       <c r="D2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="11" t="n">
+      <c r="E2" s="11">
         <v>80</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="14">
         <v>44176</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="16" t="n">
+      <c r="H2" s="16">
         <v>120344307</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="3" t="n">
+      <c r="J2" s="3">
         <v>100</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
@@ -1981,29 +2306,29 @@
       <c r="D3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="18" t="n">
+      <c r="E3" s="18">
         <v>80</v>
       </c>
-      <c r="F3" s="21" t="n">
+      <c r="F3" s="21">
         <v>44176</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="22" t="n">
+      <c r="H3" s="22">
         <v>120344364</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="3">
         <v>100</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
@@ -2016,29 +2341,29 @@
       <c r="D4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="18" t="n">
+      <c r="E4" s="18">
         <v>74</v>
       </c>
-      <c r="F4" s="21" t="n">
+      <c r="F4" s="21">
         <v>44146</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="22" t="n">
+      <c r="H4" s="22">
         <v>120344112</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="3">
         <v>100</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
@@ -2051,29 +2376,29 @@
       <c r="D5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="18" t="n">
-        <v>100</v>
-      </c>
-      <c r="F5" s="21" t="n">
+      <c r="E5" s="18">
+        <v>100</v>
+      </c>
+      <c r="F5" s="21">
         <v>44176</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="22" t="n">
+      <c r="H5" s="22">
         <v>120344352</v>
       </c>
       <c r="I5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="3">
         <v>100</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>11</v>
       </c>
@@ -2086,29 +2411,29 @@
       <c r="D6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="18" t="n">
+      <c r="E6" s="18">
         <v>60</v>
       </c>
-      <c r="F6" s="21" t="n">
+      <c r="F6" s="21">
         <v>44176</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="22" t="n">
+      <c r="H6" s="22">
         <v>120344308</v>
       </c>
       <c r="I6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="3">
         <v>100</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
@@ -2121,29 +2446,29 @@
       <c r="D7" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="18" t="n">
+      <c r="E7" s="18">
         <v>90</v>
       </c>
-      <c r="F7" s="21" t="n">
+      <c r="F7" s="21">
         <v>44176</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="22" t="n">
+      <c r="H7" s="22">
         <v>120344352</v>
       </c>
       <c r="I7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="3" t="n">
+      <c r="J7" s="3">
         <v>100</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>11</v>
       </c>
@@ -2159,26 +2484,26 @@
       <c r="E8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="21" t="n">
+      <c r="F8" s="21">
         <v>44146</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="22" t="n">
+      <c r="H8" s="22">
         <v>120344094</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="J8" s="3">
         <v>100</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>11</v>
       </c>
@@ -2191,29 +2516,29 @@
       <c r="D9" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="18" t="n">
+      <c r="E9" s="18">
         <v>105</v>
       </c>
-      <c r="F9" s="21" t="n">
+      <c r="F9" s="21">
         <v>44176</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="22" t="n">
+      <c r="H9" s="22">
         <v>120344255</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="3">
         <v>200</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
@@ -2226,29 +2551,29 @@
       <c r="D10" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="18" t="n">
+      <c r="E10" s="18">
         <v>80</v>
       </c>
-      <c r="F10" s="21" t="n">
+      <c r="F10" s="21">
         <v>44176</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="22" t="n">
+      <c r="H10" s="22">
         <v>120344196</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="3" t="n">
+      <c r="J10" s="3">
         <v>100</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>11</v>
       </c>
@@ -2261,29 +2586,29 @@
       <c r="D11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="18" t="n">
+      <c r="E11" s="18">
         <v>80</v>
       </c>
-      <c r="F11" s="21" t="n">
+      <c r="F11" s="21">
         <v>44176</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="22" t="n">
+      <c r="H11" s="22">
         <v>120344195</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="3" t="n">
+      <c r="J11" s="3">
         <v>100</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>11</v>
       </c>
@@ -2296,29 +2621,29 @@
       <c r="D12" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="18" t="n">
+      <c r="E12" s="18">
         <v>80</v>
       </c>
-      <c r="F12" s="21" t="n">
+      <c r="F12" s="21">
         <v>44176</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="22" t="n">
+      <c r="H12" s="22">
         <v>120344184</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="3" t="n">
+      <c r="J12" s="3">
         <v>100</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:11" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>45</v>
       </c>
@@ -2331,29 +2656,29 @@
       <c r="D13" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="18" t="n">
+      <c r="E13" s="18">
         <v>80</v>
       </c>
-      <c r="F13" s="21" t="n">
+      <c r="F13" s="21">
         <v>44176</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="22" t="n">
+      <c r="H13" s="22">
         <v>120344135</v>
       </c>
       <c r="I13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="3" t="n">
+      <c r="J13" s="3">
         <v>100</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>11</v>
       </c>
@@ -2366,29 +2691,29 @@
       <c r="D14" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="18" t="n">
+      <c r="E14" s="18">
         <v>75</v>
       </c>
-      <c r="F14" s="21" t="n">
+      <c r="F14" s="21">
         <v>44176</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="22" t="n">
+      <c r="H14" s="22">
         <v>120344129</v>
       </c>
       <c r="I14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="3" t="n">
+      <c r="J14" s="3">
         <v>100</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
@@ -2404,26 +2729,26 @@
       <c r="E15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="21" t="n">
+      <c r="F15" s="21">
         <v>44176</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="22" t="n">
+      <c r="H15" s="22">
         <v>120344369</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="3" t="n">
+      <c r="J15" s="3">
         <v>100</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>11</v>
       </c>
@@ -2436,29 +2761,29 @@
       <c r="D16" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="18" t="n">
+      <c r="E16" s="18">
         <v>85</v>
       </c>
-      <c r="F16" s="21" t="n">
+      <c r="F16" s="21">
         <v>44176</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="22" t="n">
+      <c r="H16" s="22">
         <v>120344330</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="3" t="n">
+      <c r="J16" s="3">
         <v>100</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>11</v>
       </c>
@@ -2471,29 +2796,29 @@
       <c r="D17" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="18" t="n">
+      <c r="E17" s="18">
         <v>95</v>
       </c>
-      <c r="F17" s="21" t="n">
+      <c r="F17" s="21">
         <v>44146</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="22" t="n">
+      <c r="H17" s="22">
         <v>120344100</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="3" t="n">
+      <c r="J17" s="3">
         <v>100</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>11</v>
       </c>
@@ -2506,29 +2831,29 @@
       <c r="D18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="18" t="n">
+      <c r="E18" s="18">
         <v>120</v>
       </c>
-      <c r="F18" s="21" t="n">
+      <c r="F18" s="21">
         <v>44176</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="22" t="n">
+      <c r="H18" s="22">
         <v>120344340</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="3" t="n">
+      <c r="J18" s="3">
         <v>100</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>11</v>
       </c>
@@ -2544,26 +2869,26 @@
       <c r="E19" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="21" t="n">
+      <c r="F19" s="21">
         <v>44176</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="22" t="n">
+      <c r="H19" s="22">
         <v>120344295</v>
       </c>
       <c r="I19" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="3" t="n">
+      <c r="J19" s="3">
         <v>100</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>11</v>
       </c>
@@ -2576,29 +2901,29 @@
       <c r="D20" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="18" t="n">
+      <c r="E20" s="18">
         <v>173</v>
       </c>
-      <c r="F20" s="21" t="n">
+      <c r="F20" s="21">
         <v>44176</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="22" t="n">
+      <c r="H20" s="22">
         <v>120344266</v>
       </c>
       <c r="I20" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="J20" s="3" t="n">
+      <c r="J20" s="3">
         <v>200</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>11</v>
       </c>
@@ -2614,26 +2939,26 @@
       <c r="E21" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="21" t="n">
+      <c r="F21" s="21">
         <v>44176</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="22" t="n">
+      <c r="H21" s="22">
         <v>120344324</v>
       </c>
       <c r="I21" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="J21" s="3" t="n">
+      <c r="J21" s="3">
         <v>200</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>11</v>
       </c>
@@ -2646,29 +2971,29 @@
       <c r="D22" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="18" t="n">
-        <v>100</v>
-      </c>
-      <c r="F22" s="21" t="n">
+      <c r="E22" s="18">
+        <v>100</v>
+      </c>
+      <c r="F22" s="21">
         <v>44176</v>
       </c>
       <c r="G22" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="22" t="n">
+      <c r="H22" s="22">
         <v>120344293</v>
       </c>
       <c r="I22" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="J22" s="3" t="n">
+      <c r="J22" s="3">
         <v>100</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>11</v>
       </c>
@@ -2681,29 +3006,29 @@
       <c r="D23" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="18" t="n">
+      <c r="E23" s="18">
         <v>120</v>
       </c>
-      <c r="F23" s="21" t="n">
+      <c r="F23" s="21">
         <v>44176</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="22" t="n">
+      <c r="H23" s="22">
         <v>120344333</v>
       </c>
       <c r="I23" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="J23" s="3" t="n">
+      <c r="J23" s="3">
         <v>100</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>11</v>
       </c>
@@ -2716,29 +3041,29 @@
       <c r="D24" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="18" t="n">
+      <c r="E24" s="18">
         <v>60</v>
       </c>
-      <c r="F24" s="21" t="n">
+      <c r="F24" s="21">
         <v>44176</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="22" t="n">
+      <c r="H24" s="22">
         <v>120344254</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="J24" s="3" t="n">
+      <c r="J24" s="3">
         <v>100</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>11</v>
       </c>
@@ -2754,26 +3079,26 @@
       <c r="E25" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F25" s="21" t="n">
+      <c r="F25" s="21">
         <v>44146</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="22" t="n">
+      <c r="H25" s="22">
         <v>120343858</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J25" s="3" t="n">
+      <c r="J25" s="3">
         <v>100</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>11</v>
       </c>
@@ -2786,29 +3111,29 @@
       <c r="D26" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="18" t="n">
+      <c r="E26" s="18">
         <v>73</v>
       </c>
-      <c r="F26" s="21" t="n">
+      <c r="F26" s="21">
         <v>44176</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="22" t="n">
+      <c r="H26" s="22">
         <v>120344345</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J26" s="3" t="n">
+      <c r="J26" s="3">
         <v>100</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>11</v>
       </c>
@@ -2821,29 +3146,29 @@
       <c r="D27" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="18" t="n">
+      <c r="E27" s="18">
         <v>58</v>
       </c>
-      <c r="F27" s="21" t="n">
+      <c r="F27" s="21">
         <v>44176</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="22" t="n">
+      <c r="H27" s="22">
         <v>120344250</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="J27" s="3" t="n">
+      <c r="J27" s="3">
         <v>100</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>11</v>
       </c>
@@ -2859,26 +3184,26 @@
       <c r="E28" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="21" t="n">
+      <c r="F28" s="21">
         <v>44176</v>
       </c>
       <c r="G28" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="22" t="n">
+      <c r="H28" s="22">
         <v>120344320</v>
       </c>
       <c r="I28" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="J28" s="3" t="n">
+      <c r="J28" s="3">
         <v>100</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>11</v>
       </c>
@@ -2894,26 +3219,26 @@
       <c r="E29" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="21" t="n">
+      <c r="F29" s="21">
         <v>44146</v>
       </c>
       <c r="G29" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="22" t="n">
+      <c r="H29" s="22">
         <v>120343945</v>
       </c>
       <c r="I29" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="J29" s="3" t="n">
+      <c r="J29" s="3">
         <v>100</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>11</v>
       </c>
@@ -2926,29 +3251,29 @@
       <c r="D30" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="18" t="n">
+      <c r="E30" s="18">
         <v>60</v>
       </c>
-      <c r="F30" s="21" t="n">
+      <c r="F30" s="21">
         <v>44176</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="22" t="n">
+      <c r="H30" s="22">
         <v>120344313</v>
       </c>
       <c r="I30" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="3" t="n">
+      <c r="J30" s="3">
         <v>100</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>11</v>
       </c>
@@ -2964,26 +3289,26 @@
       <c r="E31" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F31" s="21" t="n">
+      <c r="F31" s="21">
         <v>44176</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="22" t="n">
+      <c r="H31" s="22">
         <v>120344186</v>
       </c>
       <c r="I31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="J31" s="3" t="n">
+      <c r="J31" s="3">
         <v>100</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:11" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>11</v>
       </c>
@@ -2996,29 +3321,29 @@
       <c r="D32" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="18" t="n">
+      <c r="E32" s="18">
         <v>73</v>
       </c>
-      <c r="F32" s="21" t="n">
+      <c r="F32" s="21">
         <v>44176</v>
       </c>
       <c r="G32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="22" t="n">
+      <c r="H32" s="22">
         <v>120344345</v>
       </c>
       <c r="I32" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J32" s="3" t="n">
+      <c r="J32" s="3">
         <v>100</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:11" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>11</v>
       </c>
@@ -3031,22 +3356,22 @@
       <c r="D33" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="18" t="n">
+      <c r="E33" s="18">
         <v>170</v>
       </c>
-      <c r="F33" s="21" t="n">
+      <c r="F33" s="21">
         <v>44146</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="22" t="n">
+      <c r="H33" s="22">
         <v>120343922</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="J33" s="3" t="n">
+      <c r="J33" s="3">
         <v>200</v>
       </c>
       <c r="K33" s="3" t="s">
@@ -3054,14 +3379,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>

</xml_diff>

<commit_message>
working zcc code again, fixed infinite loop bug --> split order when width and height are larger than grid width
</commit_message>
<xml_diff>
--- a/tests/test_paklijsten/paklijst1.xlsx
+++ b/tests/test_paklijsten/paklijst1.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\HDS\2d_rectangle_packing\tests\test_paklijsten\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9438AE-E464-462F-B5BA-2C367C761DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="paklijst_zonder_opmaak" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Paklijst" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="paklijst_zonder_opmaak" sheetId="1" r:id="rId1"/>
+    <sheet name="Paklijst" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,64 +26,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="110">
-  <si>
-    <t xml:space="preserve">Aantal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omschrijving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Breedte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lengte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orderdatum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coupage/Batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ordernummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Klantnaam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rolbreedte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kleur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kokos</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="111">
+  <si>
+    <t>Aantal</t>
+  </si>
+  <si>
+    <t>Merk</t>
+  </si>
+  <si>
+    <t>Omschrijving</t>
+  </si>
+  <si>
+    <t>Breedte</t>
+  </si>
+  <si>
+    <t>Lengte</t>
+  </si>
+  <si>
+    <t>Orderdatum</t>
+  </si>
+  <si>
+    <t>Coupage/Batch</t>
+  </si>
+  <si>
+    <t>Ordernummer</t>
+  </si>
+  <si>
+    <t>Klantnaam</t>
+  </si>
+  <si>
+    <t>Rolbreedte</t>
+  </si>
+  <si>
+    <t>Kleur</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Kokos</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet 50 x 80 cm_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Dings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">antraciet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. van de Venn</t>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>Mevr. Dings</t>
+  </si>
+  <si>
+    <t>antraciet</t>
+  </si>
+  <si>
+    <t>Dhr. van de Venn</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -89,10 +94,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. Siebers</t>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Dhr. Siebers</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -101,10 +106,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tandartsenpraktijk Jansen</t>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Tandartsenpraktijk Jansen</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -115,10 +120,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. van Hees</t>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Mevr. van Hees</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -129,7 +134,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">85</t>
+    <t>85</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -138,13 +143,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">98,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. Edens</t>
+    <t>98,5</t>
+  </si>
+  <si>
+    <t>81,5</t>
+  </si>
+  <si>
+    <t>Dhr. Edens</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Antraciet op maat_x000D_
@@ -153,39 +158,39 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">197</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lash &amp; Brow Bar</t>
+    <t>197</t>
+  </si>
+  <si>
+    <t>Lash &amp; Brow Bar</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Grijs 60 x 80 cm_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Boers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grijs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. De Groot</t>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Mevr. Boers</t>
+  </si>
+  <si>
+    <t>grijs</t>
+  </si>
+  <si>
+    <t>Mevr. De Groot</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel 60 x 80 cm_x000D_
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Beugels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">naturel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
+    <t>Mevr. Beugels</t>
+  </si>
+  <si>
+    <t>naturel</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel 60 x 80 cm_x000D_
@@ -193,7 +198,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Dhr. Venhorst</t>
+    <t>Dhr. Venhorst</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -202,10 +207,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. Van der Zwaag</t>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Dhr. Van der Zwaag</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -214,13 +219,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. de Ruijter</t>
+    <t>101</t>
+  </si>
+  <si>
+    <t>93,5</t>
+  </si>
+  <si>
+    <t>Mevr. de Ruijter</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -229,10 +234,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Valk</t>
+    <t>103</t>
+  </si>
+  <si>
+    <t>Mevr. Valk</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -241,10 +246,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Veltman</t>
+    <t>160</t>
+  </si>
+  <si>
+    <t>Mevr. Veltman</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -255,7 +260,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Groen</t>
+    <t>Mevr. Groen</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -264,13 +269,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">91,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. De vuyst</t>
+    <t>91,2</t>
+  </si>
+  <si>
+    <t>92,3</t>
+  </si>
+  <si>
+    <t>Dhr. De vuyst</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -279,10 +284,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Bongertman</t>
+    <t>127</t>
+  </si>
+  <si>
+    <t>Mevr. Bongertman</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Naturel op maat_x000D_
@@ -291,13 +296,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">141,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. de Bruin</t>
+    <t>141,3</t>
+  </si>
+  <si>
+    <t>60,3</t>
+  </si>
+  <si>
+    <t>Mevr. de Bruin</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -306,10 +311,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Zeevat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zwart</t>
+    <t>Mevr. Zeevat</t>
+  </si>
+  <si>
+    <t>zwart</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -318,7 +323,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Michelle’s schoonmaakbedrijf</t>
+    <t>Michelle’s schoonmaakbedrijf</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -327,7 +332,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Cortlever</t>
+    <t>Mevr. Cortlever</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -336,10 +341,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">72,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. wiebenga</t>
+    <t>72,5</t>
+  </si>
+  <si>
+    <t>Mevr. wiebenga</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -350,10 +355,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Dubois</t>
+    <t>113</t>
+  </si>
+  <si>
+    <t>Mevr. Dubois</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -362,10 +367,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">38,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Thys</t>
+    <t>38,3</t>
+  </si>
+  <si>
+    <t>Mevr. Thys</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -376,13 +381,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhr. Rops</t>
+    <t>68</t>
+  </si>
+  <si>
+    <t>104,5</t>
+  </si>
+  <si>
+    <t>Dhr. Rops</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -393,13 +398,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Haan</t>
+    <t>78</t>
+  </si>
+  <si>
+    <t>48,5</t>
+  </si>
+  <si>
+    <t>Mevr. Haan</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -408,7 +413,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mevr. Huisman</t>
+    <t>Mevr. Huisman</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -417,13 +422,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">86,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Pijnenburg</t>
+    <t>86,5</t>
+  </si>
+  <si>
+    <t>48,3</t>
+  </si>
+  <si>
+    <t>Mevr. Pijnenburg</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -432,7 +437,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">87</t>
+    <t>87</t>
   </si>
   <si>
     <t xml:space="preserve">Kokosmat Zwart op maat_x000D_
@@ -443,25 +448,26 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mevr. Harsch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Batch/Coupage</t>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Mevr. Harsch</t>
+  </si>
+  <si>
+    <t>Batch/Coupage</t>
+  </si>
+  <si>
+    <t>Materiaal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -471,28 +477,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -509,1396 +500,1729 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:K33" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:K33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabel1" displayName="Tabel1" ref="A1:K33" totalsRowShown="0">
+  <autoFilter ref="A1:K33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="Aantal"/>
-    <tableColumn id="2" name="Merk"/>
-    <tableColumn id="3" name="Omschrijving"/>
-    <tableColumn id="4" name="Breedte"/>
-    <tableColumn id="5" name="Lengte"/>
-    <tableColumn id="6" name="Orderdatum"/>
-    <tableColumn id="7" name="Batch/Coupage"/>
-    <tableColumn id="8" name="Ordernummer"/>
-    <tableColumn id="9" name="Klantnaam"/>
-    <tableColumn id="10" name="Rolbreedte"/>
-    <tableColumn id="11" name="Kleur"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Aantal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Merk"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Omschrijving"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Breedte"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Lengte"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Orderdatum"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Batch/Coupage"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ordernummer"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Klantnaam"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Rolbreedte"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Kleur"/>
   </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
+    <col min="1" max="1" width="6.5703125"/>
+    <col min="2" max="2" width="6.140625"/>
+    <col min="3" max="3" width="53.85546875"/>
+    <col min="4" max="4" width="8"/>
+    <col min="5" max="5" width="6.85546875"/>
+    <col min="6" max="6" width="11.5703125"/>
+    <col min="7" max="7" width="14.28515625"/>
+    <col min="8" max="8" width="13.5703125"/>
+    <col min="9" max="9" width="27.85546875"/>
+    <col min="10" max="10" width="10.85546875"/>
+    <col min="11" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="L1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>80</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="0" t="n">
+      <c r="F2">
+        <v>44176</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
         <v>120344307</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K2" s="0" t="s">
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>80</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="F3">
+        <v>44176</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
         <v>120344364</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K3" s="0" t="s">
+      <c r="J3">
+        <v>100</v>
+      </c>
+      <c r="K3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>74</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>44146</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
         <v>120344112</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K4" s="0" t="s">
+      <c r="J4">
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="0" t="n">
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>44176</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
         <v>120344352</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K5" s="0" t="s">
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="K5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>60</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="0" t="n">
+      <c r="F6">
+        <v>44176</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
         <v>120344308</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K6" s="0" t="s">
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="K6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="L6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>90</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="F7">
+        <v>44176</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
         <v>120344352</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K7" s="0" t="s">
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="0" t="s">
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8">
         <v>44146</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
         <v>120344094</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K8" s="0" t="s">
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9">
         <v>105</v>
       </c>
-      <c r="F9" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="0" t="n">
+      <c r="F9">
+        <v>44176</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
         <v>120344255</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9">
         <v>200</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="L9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10">
         <v>80</v>
       </c>
-      <c r="F10" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="0" t="n">
+      <c r="F10">
+        <v>44176</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10">
         <v>120344196</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K10" s="0" t="s">
+      <c r="J10">
+        <v>100</v>
+      </c>
+      <c r="K10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="L10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11">
         <v>80</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="0" t="n">
+      <c r="F11">
+        <v>44176</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
         <v>120344195</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K11" s="0" t="s">
+      <c r="J11">
+        <v>100</v>
+      </c>
+      <c r="K11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="L11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12">
         <v>80</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="0" t="n">
+      <c r="F12">
+        <v>44176</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12">
         <v>120344184</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K12" s="0" t="s">
+      <c r="J12">
+        <v>100</v>
+      </c>
+      <c r="K12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="L12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13">
         <v>80</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="0" t="n">
+      <c r="F13">
+        <v>44176</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13">
         <v>120344135</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K13" s="0" t="s">
+      <c r="J13">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="L13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14">
         <v>75</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="0" t="n">
+      <c r="F14">
+        <v>44176</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14">
         <v>120344129</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K14" s="0" t="s">
+      <c r="J14">
+        <v>100</v>
+      </c>
+      <c r="K14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="L14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="0" t="n">
+      <c r="F15">
+        <v>44176</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15">
         <v>120344369</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K15" s="0" t="s">
+      <c r="J15">
+        <v>100</v>
+      </c>
+      <c r="K15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="L15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16">
         <v>85</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="0" t="n">
+      <c r="F16">
+        <v>44176</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16">
         <v>120344330</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K16" s="0" t="s">
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="L16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17">
         <v>95</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17">
         <v>44146</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="0" t="n">
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17">
         <v>120344100</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K17" s="0" t="s">
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="L17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18">
         <v>120</v>
       </c>
-      <c r="F18" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="0" t="n">
+      <c r="F18">
+        <v>44176</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18">
         <v>120344340</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K18" s="0" t="s">
+      <c r="J18">
+        <v>100</v>
+      </c>
+      <c r="K18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="L18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="0" t="n">
+      <c r="F19">
+        <v>44176</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
         <v>120344295</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K19" s="0" t="s">
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="0" t="s">
+      <c r="L19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20">
         <v>173</v>
       </c>
-      <c r="F20" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="0" t="n">
+      <c r="F20">
+        <v>44176</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20">
         <v>120344266</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" t="s">
         <v>69</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20">
         <v>200</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="K20" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="L20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="0" t="n">
+      <c r="F21">
+        <v>44176</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21">
         <v>120344324</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" t="s">
         <v>73</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21">
         <v>200</v>
       </c>
-      <c r="K21" s="0" t="s">
+      <c r="K21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="0" t="s">
+      <c r="L21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="0" t="n">
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>44176</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22">
         <v>120344293</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="I22" t="s">
         <v>75</v>
       </c>
-      <c r="J22" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K22" s="0" t="s">
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="K22" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="0" t="s">
+      <c r="L22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23">
         <v>120</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="0" t="n">
+      <c r="F23">
+        <v>44176</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23">
         <v>120344333</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="I23" t="s">
         <v>78</v>
       </c>
-      <c r="J23" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K23" s="0" t="s">
+      <c r="J23">
+        <v>100</v>
+      </c>
+      <c r="K23" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="0" t="s">
+      <c r="L23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24">
         <v>60</v>
       </c>
-      <c r="F24" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="0" t="n">
+      <c r="F24">
+        <v>44176</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24">
         <v>120344254</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" t="s">
         <v>80</v>
       </c>
-      <c r="J24" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K24" s="0" t="s">
+      <c r="J24">
+        <v>100</v>
+      </c>
+      <c r="K24" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="0" t="s">
+      <c r="L24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" t="s">
         <v>82</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25">
         <v>44146</v>
       </c>
-      <c r="G25" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="0" t="n">
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25">
         <v>120343858</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="I25" t="s">
         <v>83</v>
       </c>
-      <c r="J25" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K25" s="0" t="s">
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="0" t="s">
+      <c r="L25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26">
         <v>73</v>
       </c>
-      <c r="F26" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="0" t="n">
+      <c r="F26">
+        <v>44176</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26">
         <v>120344345</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I26" t="s">
         <v>86</v>
       </c>
-      <c r="J26" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K26" s="0" t="s">
+      <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="0" t="s">
+      <c r="L26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27">
         <v>58</v>
       </c>
-      <c r="F27" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="0" t="n">
+      <c r="F27">
+        <v>44176</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27">
         <v>120344250</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I27" t="s">
         <v>89</v>
       </c>
-      <c r="J27" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K27" s="0" t="s">
+      <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="K27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="0" t="s">
+      <c r="L27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="0" t="n">
+      <c r="F28">
+        <v>44176</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28">
         <v>120344320</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="I28" t="s">
         <v>93</v>
       </c>
-      <c r="J28" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K28" s="0" t="s">
+      <c r="J28">
+        <v>100</v>
+      </c>
+      <c r="K28" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="L28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29">
         <v>44146</v>
       </c>
-      <c r="G29" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="0" t="n">
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29">
         <v>120343945</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="I29" t="s">
         <v>97</v>
       </c>
-      <c r="J29" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K29" s="0" t="s">
+      <c r="J29">
+        <v>100</v>
+      </c>
+      <c r="K29" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="0" t="s">
+      <c r="L29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30">
         <v>60</v>
       </c>
-      <c r="F30" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G30" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="0" t="n">
+      <c r="F30">
+        <v>44176</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30">
         <v>120344313</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="I30" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K30" s="0" t="s">
+      <c r="J30">
+        <v>100</v>
+      </c>
+      <c r="K30" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="0" t="s">
+      <c r="L30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" t="s">
         <v>102</v>
       </c>
-      <c r="F31" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="0" t="n">
+      <c r="F31">
+        <v>44176</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31">
         <v>120344186</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="I31" t="s">
         <v>103</v>
       </c>
-      <c r="J31" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K31" s="0" t="s">
+      <c r="J31">
+        <v>100</v>
+      </c>
+      <c r="K31" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="0" t="s">
+      <c r="L31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32">
         <v>73</v>
       </c>
-      <c r="F32" s="0" t="n">
-        <v>44176</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="0" t="n">
+      <c r="F32">
+        <v>44176</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32">
         <v>120344345</v>
       </c>
-      <c r="I32" s="0" t="s">
+      <c r="I32" t="s">
         <v>86</v>
       </c>
-      <c r="J32" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="K32" s="0" t="s">
+      <c r="J32">
+        <v>100</v>
+      </c>
+      <c r="K32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="0" t="s">
+      <c r="L32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33">
         <v>170</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33">
         <v>44146</v>
       </c>
-      <c r="G33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="0" t="n">
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33">
         <v>120343922</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="I33" t="s">
         <v>108</v>
       </c>
-      <c r="J33" s="0" t="n">
+      <c r="J33">
         <v>200</v>
       </c>
-      <c r="K33" s="0" t="s">
+      <c r="K33" t="s">
         <v>76</v>
       </c>
+      <c r="L33" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="3" width="9.04591836734694"/>
+    <col min="1" max="1" width="8" style="2"/>
+    <col min="2" max="2" width="15.7109375" style="3"/>
+    <col min="3" max="3" width="42.5703125" style="3"/>
+    <col min="4" max="4" width="9.42578125" style="4"/>
+    <col min="5" max="5" width="8.42578125" style="3"/>
+    <col min="6" max="6" width="12.85546875" style="3"/>
+    <col min="7" max="7" width="14.7109375" style="5"/>
+    <col min="8" max="8" width="14.42578125" style="5"/>
+    <col min="9" max="9" width="27.140625" style="3"/>
+    <col min="10" max="1025" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1933,7 +2257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -1946,29 +2270,29 @@
       <c r="D2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="11" t="n">
+      <c r="E2" s="11">
         <v>80</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="14">
         <v>44176</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="16" t="n">
+      <c r="H2" s="16">
         <v>120344307</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="3" t="n">
+      <c r="J2" s="3">
         <v>100</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
@@ -1981,29 +2305,29 @@
       <c r="D3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="18" t="n">
+      <c r="E3" s="18">
         <v>80</v>
       </c>
-      <c r="F3" s="21" t="n">
+      <c r="F3" s="21">
         <v>44176</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="22" t="n">
+      <c r="H3" s="22">
         <v>120344364</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="3">
         <v>100</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
@@ -2016,29 +2340,29 @@
       <c r="D4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="18" t="n">
+      <c r="E4" s="18">
         <v>74</v>
       </c>
-      <c r="F4" s="21" t="n">
+      <c r="F4" s="21">
         <v>44146</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="22" t="n">
+      <c r="H4" s="22">
         <v>120344112</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="3">
         <v>100</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>11</v>
       </c>
@@ -2051,29 +2375,29 @@
       <c r="D5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="18" t="n">
-        <v>100</v>
-      </c>
-      <c r="F5" s="21" t="n">
+      <c r="E5" s="18">
+        <v>100</v>
+      </c>
+      <c r="F5" s="21">
         <v>44176</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="22" t="n">
+      <c r="H5" s="22">
         <v>120344352</v>
       </c>
       <c r="I5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="3">
         <v>100</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>11</v>
       </c>
@@ -2086,29 +2410,29 @@
       <c r="D6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="18" t="n">
+      <c r="E6" s="18">
         <v>60</v>
       </c>
-      <c r="F6" s="21" t="n">
+      <c r="F6" s="21">
         <v>44176</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="22" t="n">
+      <c r="H6" s="22">
         <v>120344308</v>
       </c>
       <c r="I6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="3">
         <v>100</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>11</v>
       </c>
@@ -2121,29 +2445,29 @@
       <c r="D7" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="18" t="n">
+      <c r="E7" s="18">
         <v>90</v>
       </c>
-      <c r="F7" s="21" t="n">
+      <c r="F7" s="21">
         <v>44176</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="22" t="n">
+      <c r="H7" s="22">
         <v>120344352</v>
       </c>
       <c r="I7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="3" t="n">
+      <c r="J7" s="3">
         <v>100</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>11</v>
       </c>
@@ -2159,26 +2483,26 @@
       <c r="E8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="21" t="n">
+      <c r="F8" s="21">
         <v>44146</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="22" t="n">
+      <c r="H8" s="22">
         <v>120344094</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="J8" s="3">
         <v>100</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>11</v>
       </c>
@@ -2191,29 +2515,29 @@
       <c r="D9" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="18" t="n">
+      <c r="E9" s="18">
         <v>105</v>
       </c>
-      <c r="F9" s="21" t="n">
+      <c r="F9" s="21">
         <v>44176</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="22" t="n">
+      <c r="H9" s="22">
         <v>120344255</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="3">
         <v>200</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
@@ -2226,29 +2550,29 @@
       <c r="D10" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="18" t="n">
+      <c r="E10" s="18">
         <v>80</v>
       </c>
-      <c r="F10" s="21" t="n">
+      <c r="F10" s="21">
         <v>44176</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="22" t="n">
+      <c r="H10" s="22">
         <v>120344196</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="3" t="n">
+      <c r="J10" s="3">
         <v>100</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>11</v>
       </c>
@@ -2261,29 +2585,29 @@
       <c r="D11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="18" t="n">
+      <c r="E11" s="18">
         <v>80</v>
       </c>
-      <c r="F11" s="21" t="n">
+      <c r="F11" s="21">
         <v>44176</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="22" t="n">
+      <c r="H11" s="22">
         <v>120344195</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="3" t="n">
+      <c r="J11" s="3">
         <v>100</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>11</v>
       </c>
@@ -2296,29 +2620,29 @@
       <c r="D12" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="18" t="n">
+      <c r="E12" s="18">
         <v>80</v>
       </c>
-      <c r="F12" s="21" t="n">
+      <c r="F12" s="21">
         <v>44176</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="22" t="n">
+      <c r="H12" s="22">
         <v>120344184</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="3" t="n">
+      <c r="J12" s="3">
         <v>100</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:11" ht="39" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>45</v>
       </c>
@@ -2331,29 +2655,29 @@
       <c r="D13" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="18" t="n">
+      <c r="E13" s="18">
         <v>80</v>
       </c>
-      <c r="F13" s="21" t="n">
+      <c r="F13" s="21">
         <v>44176</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="22" t="n">
+      <c r="H13" s="22">
         <v>120344135</v>
       </c>
       <c r="I13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J13" s="3" t="n">
+      <c r="J13" s="3">
         <v>100</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>11</v>
       </c>
@@ -2366,29 +2690,29 @@
       <c r="D14" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="18" t="n">
+      <c r="E14" s="18">
         <v>75</v>
       </c>
-      <c r="F14" s="21" t="n">
+      <c r="F14" s="21">
         <v>44176</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="22" t="n">
+      <c r="H14" s="22">
         <v>120344129</v>
       </c>
       <c r="I14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="3" t="n">
+      <c r="J14" s="3">
         <v>100</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
@@ -2404,26 +2728,26 @@
       <c r="E15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="21" t="n">
+      <c r="F15" s="21">
         <v>44176</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="22" t="n">
+      <c r="H15" s="22">
         <v>120344369</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="3" t="n">
+      <c r="J15" s="3">
         <v>100</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>11</v>
       </c>
@@ -2436,29 +2760,29 @@
       <c r="D16" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="18" t="n">
+      <c r="E16" s="18">
         <v>85</v>
       </c>
-      <c r="F16" s="21" t="n">
+      <c r="F16" s="21">
         <v>44176</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="22" t="n">
+      <c r="H16" s="22">
         <v>120344330</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="3" t="n">
+      <c r="J16" s="3">
         <v>100</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>11</v>
       </c>
@@ -2471,29 +2795,29 @@
       <c r="D17" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="18" t="n">
+      <c r="E17" s="18">
         <v>95</v>
       </c>
-      <c r="F17" s="21" t="n">
+      <c r="F17" s="21">
         <v>44146</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="22" t="n">
+      <c r="H17" s="22">
         <v>120344100</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="3" t="n">
+      <c r="J17" s="3">
         <v>100</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>11</v>
       </c>
@@ -2506,29 +2830,29 @@
       <c r="D18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="18" t="n">
+      <c r="E18" s="18">
         <v>120</v>
       </c>
-      <c r="F18" s="21" t="n">
+      <c r="F18" s="21">
         <v>44176</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="22" t="n">
+      <c r="H18" s="22">
         <v>120344340</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="3" t="n">
+      <c r="J18" s="3">
         <v>100</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>11</v>
       </c>
@@ -2544,26 +2868,26 @@
       <c r="E19" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="21" t="n">
+      <c r="F19" s="21">
         <v>44176</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="22" t="n">
+      <c r="H19" s="22">
         <v>120344295</v>
       </c>
       <c r="I19" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="3" t="n">
+      <c r="J19" s="3">
         <v>100</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>11</v>
       </c>
@@ -2576,29 +2900,29 @@
       <c r="D20" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="18" t="n">
+      <c r="E20" s="18">
         <v>173</v>
       </c>
-      <c r="F20" s="21" t="n">
+      <c r="F20" s="21">
         <v>44176</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="22" t="n">
+      <c r="H20" s="22">
         <v>120344266</v>
       </c>
       <c r="I20" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="J20" s="3" t="n">
+      <c r="J20" s="3">
         <v>200</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>11</v>
       </c>
@@ -2614,26 +2938,26 @@
       <c r="E21" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="21" t="n">
+      <c r="F21" s="21">
         <v>44176</v>
       </c>
       <c r="G21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="22" t="n">
+      <c r="H21" s="22">
         <v>120344324</v>
       </c>
       <c r="I21" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="J21" s="3" t="n">
+      <c r="J21" s="3">
         <v>200</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>11</v>
       </c>
@@ -2646,29 +2970,29 @@
       <c r="D22" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="18" t="n">
-        <v>100</v>
-      </c>
-      <c r="F22" s="21" t="n">
+      <c r="E22" s="18">
+        <v>100</v>
+      </c>
+      <c r="F22" s="21">
         <v>44176</v>
       </c>
       <c r="G22" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="22" t="n">
+      <c r="H22" s="22">
         <v>120344293</v>
       </c>
       <c r="I22" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="J22" s="3" t="n">
+      <c r="J22" s="3">
         <v>100</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>11</v>
       </c>
@@ -2681,29 +3005,29 @@
       <c r="D23" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="18" t="n">
+      <c r="E23" s="18">
         <v>120</v>
       </c>
-      <c r="F23" s="21" t="n">
+      <c r="F23" s="21">
         <v>44176</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="22" t="n">
+      <c r="H23" s="22">
         <v>120344333</v>
       </c>
       <c r="I23" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="J23" s="3" t="n">
+      <c r="J23" s="3">
         <v>100</v>
       </c>
       <c r="K23" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>11</v>
       </c>
@@ -2716,29 +3040,29 @@
       <c r="D24" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="18" t="n">
+      <c r="E24" s="18">
         <v>60</v>
       </c>
-      <c r="F24" s="21" t="n">
+      <c r="F24" s="21">
         <v>44176</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="22" t="n">
+      <c r="H24" s="22">
         <v>120344254</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="J24" s="3" t="n">
+      <c r="J24" s="3">
         <v>100</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>11</v>
       </c>
@@ -2754,26 +3078,26 @@
       <c r="E25" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F25" s="21" t="n">
+      <c r="F25" s="21">
         <v>44146</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="22" t="n">
+      <c r="H25" s="22">
         <v>120343858</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J25" s="3" t="n">
+      <c r="J25" s="3">
         <v>100</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>11</v>
       </c>
@@ -2786,29 +3110,29 @@
       <c r="D26" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="18" t="n">
+      <c r="E26" s="18">
         <v>73</v>
       </c>
-      <c r="F26" s="21" t="n">
+      <c r="F26" s="21">
         <v>44176</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="22" t="n">
+      <c r="H26" s="22">
         <v>120344345</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J26" s="3" t="n">
+      <c r="J26" s="3">
         <v>100</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>11</v>
       </c>
@@ -2821,29 +3145,29 @@
       <c r="D27" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="18" t="n">
+      <c r="E27" s="18">
         <v>58</v>
       </c>
-      <c r="F27" s="21" t="n">
+      <c r="F27" s="21">
         <v>44176</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="22" t="n">
+      <c r="H27" s="22">
         <v>120344250</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="J27" s="3" t="n">
+      <c r="J27" s="3">
         <v>100</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>11</v>
       </c>
@@ -2859,26 +3183,26 @@
       <c r="E28" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="21" t="n">
+      <c r="F28" s="21">
         <v>44176</v>
       </c>
       <c r="G28" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="22" t="n">
+      <c r="H28" s="22">
         <v>120344320</v>
       </c>
       <c r="I28" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="J28" s="3" t="n">
+      <c r="J28" s="3">
         <v>100</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>11</v>
       </c>
@@ -2894,26 +3218,26 @@
       <c r="E29" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="21" t="n">
+      <c r="F29" s="21">
         <v>44146</v>
       </c>
       <c r="G29" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="22" t="n">
+      <c r="H29" s="22">
         <v>120343945</v>
       </c>
       <c r="I29" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="J29" s="3" t="n">
+      <c r="J29" s="3">
         <v>100</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>11</v>
       </c>
@@ -2926,29 +3250,29 @@
       <c r="D30" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="18" t="n">
+      <c r="E30" s="18">
         <v>60</v>
       </c>
-      <c r="F30" s="21" t="n">
+      <c r="F30" s="21">
         <v>44176</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="22" t="n">
+      <c r="H30" s="22">
         <v>120344313</v>
       </c>
       <c r="I30" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="3" t="n">
+      <c r="J30" s="3">
         <v>100</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>11</v>
       </c>
@@ -2964,26 +3288,26 @@
       <c r="E31" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F31" s="21" t="n">
+      <c r="F31" s="21">
         <v>44176</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="22" t="n">
+      <c r="H31" s="22">
         <v>120344186</v>
       </c>
       <c r="I31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="J31" s="3" t="n">
+      <c r="J31" s="3">
         <v>100</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:11" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>11</v>
       </c>
@@ -2996,29 +3320,29 @@
       <c r="D32" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="18" t="n">
+      <c r="E32" s="18">
         <v>73</v>
       </c>
-      <c r="F32" s="21" t="n">
+      <c r="F32" s="21">
         <v>44176</v>
       </c>
       <c r="G32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="22" t="n">
+      <c r="H32" s="22">
         <v>120344345</v>
       </c>
       <c r="I32" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J32" s="3" t="n">
+      <c r="J32" s="3">
         <v>100</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>11</v>
       </c>
@@ -3031,22 +3355,22 @@
       <c r="D33" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="18" t="n">
+      <c r="E33" s="18">
         <v>170</v>
       </c>
-      <c r="F33" s="21" t="n">
+      <c r="F33" s="21">
         <v>44146</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="22" t="n">
+      <c r="H33" s="22">
         <v>120343922</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="J33" s="3" t="n">
+      <c r="J33" s="3">
         <v>200</v>
       </c>
       <c r="K33" s="3" t="s">
@@ -3054,14 +3378,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <tableParts>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>

</xml_diff>

<commit_message>
modified test excels for Soort instead of Kleur
</commit_message>
<xml_diff>
--- a/tests/test_paklijsten/paklijst1.xlsx
+++ b/tests/test_paklijsten/paklijst1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\HDS\2d_rectangle_packing\tests\test_paklijsten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BC66CC-6F7F-49ED-83A6-3847D2D5CDF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA031B6-C276-45D1-B936-F6AF642E8962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="paklijst_zonder_opmaak" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="113">
   <si>
     <t>Aantal</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>Artikelnaam</t>
+  </si>
+  <si>
+    <t>Soort</t>
   </si>
 </sst>
 </file>
@@ -927,7 +930,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +981,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="L1" t="s">
         <v>110</v>

</xml_diff>